<commit_message>
Update Default Attack Number
Update default budget to about $50,000 and number of workstations to reflect a number of employees which corresponds to that budget based on Delloits 2020 report.
</commit_message>
<xml_diff>
--- a/AttackSimulationModel/node_inputs.xlsx
+++ b/AttackSimulationModel/node_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Models\AttackSimulation\AttackSimulationModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3CC6E9-0818-45A4-9D12-9459A07C1356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9006A15A-25BF-4180-BAA4-E2B1096464C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24015" yWindow="135" windowWidth="23715" windowHeight="14760" xr2:uid="{2E34376E-5056-4BF7-A421-5DDCB46FDBC9}"/>
+    <workbookView xWindow="-26445" yWindow="675" windowWidth="23715" windowHeight="14760" xr2:uid="{2E34376E-5056-4BF7-A421-5DDCB46FDBC9}"/>
   </bookViews>
   <sheets>
     <sheet name="node_inputs" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +485,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>500</v>
+        <v>25</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>

</xml_diff>